<commit_message>
Tidy up some formatting, use high res graph images, move section about privacy loss differentiation to theoretical development section
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\4thYearProject\IIB-Project-Final-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBBF89C-1DD6-414E-A82D-491D5190629B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0BB9FE-EB67-459B-99B3-1C343CB99C08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="9705" xr2:uid="{81DE1D21-D6D1-43F5-A4CE-E2015F0A1D98}"/>
   </bookViews>
@@ -2673,13 +2673,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>24318</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>110043</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3008,8 +3008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC229F44-05F6-4C04-8FCF-16D4303E0E94}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" topLeftCell="H19" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>